<commit_message>
Adding responsibilities carried out by each team member
</commit_message>
<xml_diff>
--- a/ACA Project Plan & Work Distribution.xlsx
+++ b/ACA Project Plan & Work Distribution.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ranja\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ranjan\UC Denver\Sem 2\CSCI 5593 - Advanced Computer Architecture\git\CSCI-5593_Advanced_Computer_Architecture\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{85E63024-CA68-489C-A684-0BB42A695A74}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{72EE2BB8-2226-426F-B020-ADF49D8775D4}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE5A0F6F-2C40-4E6C-8A88-75CAD136D892}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F746563E-E363-4F78-9DC7-F982FD45D4D4}"/>
+    <workbookView xWindow="60" yWindow="24" windowWidth="22980" windowHeight="12336" activeTab="1" xr2:uid="{F746563E-E363-4F78-9DC7-F982FD45D4D4}"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="2" r:id="rId1"/>
+    <sheet name="Responsibilities" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
   <si>
     <t>Combine multiple sets into partitions</t>
   </si>
@@ -88,13 +89,28 @@
   </si>
   <si>
     <t>Owner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                                </t>
+  </si>
+  <si>
+    <t>Rohan Hulsure :- Rohan was responsible for implementation of module of switching policies and implementation of promotion policy. He also identified the way gem5 can be integrated with SPEC CPU2017 benchmark, compiled libraries of SPEC CPU2017 and prepared script for gem5 by which policy can be evaluated. He also has contribution in preparing presentations for research and project. Rohan made sure that each task was completed at regular checkpoints.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vatsal Vador :- Vatsal also was involved in research for tool and module for implementation. Vatsal was responsible for implementation for the logic for task ‘At every cache access, calculate total of priority values in each partition and update all necessary priority values (GTRs, preGTRs, PTRs , prePTRs) and implementation of Demotion Policy. He also had contribution in documentation of project work (Project Report). Vatsal had on more responsibility of testing each module of the project.       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Piyush Deshpande :-  Piyush was responsible for the implementation of logic for the task ‘At every set interval, check fluctuations of the total of priority values in all partitions and then switch policies’ and implementation for Selection Policy. He also had contribution in documentation of project work (Project Report), testing end to end functionality and code optimization for complete project. </t>
+  </si>
+  <si>
+    <t>Ranjan Raut :-  Ranjan was involved in research for tool and module for implementation and Identified the way to implement policy in adherence to the framework of simulator. He also implemented code for Combining multiple sets into partitions, Insertion Policy and was also involved in performance evaluation of policy. He also contributed into preparing presentations for research and project. Ranjan reviewed complete code for the project just to ensure the functionality if implemented correctly.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -109,6 +125,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -131,7 +153,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -144,6 +166,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -461,7 +486,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A962EB2D-A4A3-40FD-BE44-1427483AFC88}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
@@ -608,4 +633,51 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{380FEC63-70DC-483F-AA5D-CD97C6EAEA39}">
+  <dimension ref="A1:A7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="5"/>
+    </row>
+    <row r="3" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="5"/>
+    </row>
+    <row r="5" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>